<commit_message>
Fix: Log, Attendance, Schedule, Login, Class
</commit_message>
<xml_diff>
--- a/SEP490_API/wwwroot/Templates/template_schedule.xlsx
+++ b/SEP490_API/wwwroot/Templates/template_schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repo\SEP490_BE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repo\SEP490_BE\SEP490_API\wwwroot\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF29C63-634F-4A0E-AF43-9F454BA3CED0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A74777-DB7E-4DF0-ADE2-C02C5A0807A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1125" windowWidth="29040" windowHeight="15720" xr2:uid="{1217BF2B-6CD0-4A14-B2A5-7D8E68CE3733}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="56">
   <si>
     <t>Năm học</t>
   </si>
@@ -164,9 +164,6 @@
     <t>gdqpan</t>
   </si>
   <si>
-    <t>homeroomteacher</t>
-  </si>
-  <si>
     <t>Ngày bắt đầu</t>
   </si>
   <si>
@@ -195,6 +192,18 @@
   </si>
   <si>
     <t>16/09/2024</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>homeroomteacher12</t>
+  </si>
+  <si>
+    <t>homeroomteacher23</t>
+  </si>
+  <si>
+    <t>homeroomteacher34</t>
   </si>
 </sst>
 </file>
@@ -556,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10289981-871F-4D91-BE02-DF222E18DE84}">
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,20 +597,20 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -651,7 +660,7 @@
         <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -761,7 +770,7 @@
         <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -772,7 +781,7 @@
         <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -783,7 +792,7 @@
         <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -967,21 +976,21 @@
     <row r="35" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" s="1"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B38" t="s">
         <v>15</v>
@@ -1031,7 +1040,7 @@
         <v>45</v>
       </c>
       <c r="C42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1130,7 +1139,7 @@
         <v>15</v>
       </c>
       <c r="C51" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -1141,7 +1150,7 @@
         <v>15</v>
       </c>
       <c r="C52" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -1152,7 +1161,7 @@
         <v>15</v>
       </c>
       <c r="C53" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -1336,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85068519-3CC4-41DA-B503-13258ADA06CA}">
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51:C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1355,7 +1364,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1368,20 +1377,20 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -1431,7 +1440,7 @@
         <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1541,7 +1550,7 @@
         <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1552,7 +1561,7 @@
         <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1563,7 +1572,7 @@
         <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1747,21 +1756,21 @@
     <row r="35" spans="1:5" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" s="1"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B38" t="s">
         <v>15</v>
@@ -1811,7 +1820,7 @@
         <v>45</v>
       </c>
       <c r="C42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1910,7 +1919,7 @@
         <v>15</v>
       </c>
       <c r="C51" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -1921,7 +1930,7 @@
         <v>15</v>
       </c>
       <c r="C52" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -1932,7 +1941,7 @@
         <v>15</v>
       </c>
       <c r="C53" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -2116,8 +2125,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99FB273F-AC51-4F53-BED0-5EF6C8B760BC}">
   <dimension ref="A1:H65"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C51" sqref="C51:C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2135,7 +2144,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2148,20 +2157,20 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -2211,7 +2220,7 @@
         <v>45</v>
       </c>
       <c r="C10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2321,7 +2330,7 @@
         <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -2332,7 +2341,7 @@
         <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -2343,7 +2352,7 @@
         <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -2527,21 +2536,21 @@
     <row r="35" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" s="1"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B38" t="s">
         <v>15</v>
@@ -2591,7 +2600,7 @@
         <v>45</v>
       </c>
       <c r="C42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -2690,7 +2699,7 @@
         <v>15</v>
       </c>
       <c r="C51" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -2701,7 +2710,7 @@
         <v>15</v>
       </c>
       <c r="C52" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -2712,7 +2721,7 @@
         <v>15</v>
       </c>
       <c r="C53" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix: Update not require password
</commit_message>
<xml_diff>
--- a/SEP490_API/wwwroot/Templates/template_schedule.xlsx
+++ b/SEP490_API/wwwroot/Templates/template_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repo\SEP490_BE\SEP490_API\wwwroot\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A74777-DB7E-4DF0-ADE2-C02C5A0807A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39524B87-1065-4379-87F7-D0187583C8CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1125" windowWidth="29040" windowHeight="15720" xr2:uid="{1217BF2B-6CD0-4A14-B2A5-7D8E68CE3733}"/>
   </bookViews>
@@ -566,7 +566,7 @@
   <dimension ref="A1:H65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>